<commit_message>
Working on final project
</commit_message>
<xml_diff>
--- a/projects/project-7-final/data/housing_2020.xlsx
+++ b/projects/project-7-final/data/housing_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
   <si>
     <t>region</t>
   </si>
@@ -321,9 +321,6 @@
     <t>домохозяйства, не собирающиеся улучшать свои жилищные условия</t>
   </si>
   <si>
-    <t>…*</t>
-  </si>
-  <si>
     <t>Название таблицы 1</t>
   </si>
   <si>
@@ -413,7 +410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -428,42 +425,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,26 +474,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,22 +510,22 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -537,25 +534,25 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -578,8 +575,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
@@ -779,12 +776,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -816,10 +813,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1058,12 +1055,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1367,10 +1364,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3933,9 +3930,7 @@
       <c r="E3" s="5">
         <v>0</v>
       </c>
-      <c r="F3" t="s" s="4">
-        <v>102</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -7002,33 +6997,33 @@
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
       <c r="A1" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s" s="9">
         <v>103</v>
       </c>
-      <c r="B1" t="s" s="9">
+      <c r="C1" t="s" s="4">
         <v>104</v>
-      </c>
-      <c r="C1" t="s" s="4">
-        <v>105</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s" s="9">
         <v>106</v>
       </c>
-      <c r="B2" t="s" s="9">
+      <c r="C2" t="s" s="10">
         <v>107</v>
-      </c>
-      <c r="C2" t="s" s="10">
-        <v>108</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
@@ -7037,7 +7032,7 @@
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
@@ -7060,10 +7055,10 @@
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s" s="9">
         <v>111</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>112</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -7071,10 +7066,10 @@
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s" s="17">
         <v>113</v>
-      </c>
-      <c r="B8" t="s" s="17">
-        <v>114</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>

</xml_diff>